<commit_message>
Added Entity and Org creation
</commit_message>
<xml_diff>
--- a/TestingFramework/TestData/testInput.xlsx
+++ b/TestingFramework/TestData/testInput.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="187">
   <si>
     <t>Customer Name</t>
   </si>
@@ -114,12 +115,6 @@
     <t>Text</t>
   </si>
   <si>
-    <t>public static String sUrl = "http://192.168.1.55:7070/kagami-studio/auth/signin";</t>
-  </si>
-  <si>
-    <t>as per sheet 4 old one working</t>
-  </si>
-  <si>
     <t>Default Attribute</t>
   </si>
   <si>
@@ -448,6 +443,144 @@
   </si>
   <si>
     <t>Business Process2</t>
+  </si>
+  <si>
+    <t>DefaultValue</t>
+  </si>
+  <si>
+    <t>Sample Value1</t>
+  </si>
+  <si>
+    <t>Sample Value2</t>
+  </si>
+  <si>
+    <t>Sample Value3</t>
+  </si>
+  <si>
+    <t>Sample Value4</t>
+  </si>
+  <si>
+    <t>Sample Value5</t>
+  </si>
+  <si>
+    <t>Sample Value6</t>
+  </si>
+  <si>
+    <t>Sample Value7</t>
+  </si>
+  <si>
+    <t>Sample Value8</t>
+  </si>
+  <si>
+    <t>Sample Value9</t>
+  </si>
+  <si>
+    <t>Sample Value16</t>
+  </si>
+  <si>
+    <t>Sample Value 17</t>
+  </si>
+  <si>
+    <t>Sample Value 18</t>
+  </si>
+  <si>
+    <t>Sample Value 19</t>
+  </si>
+  <si>
+    <t>Sample Value 20</t>
+  </si>
+  <si>
+    <t>Sample Value 21</t>
+  </si>
+  <si>
+    <t>Sample Value 26</t>
+  </si>
+  <si>
+    <t>Sample Value 27</t>
+  </si>
+  <si>
+    <t>Sample Value 28</t>
+  </si>
+  <si>
+    <t>Sample Value 29</t>
+  </si>
+  <si>
+    <t>Sample Value 30</t>
+  </si>
+  <si>
+    <t>Sample Value 31</t>
+  </si>
+  <si>
+    <t>Sample Value 32</t>
+  </si>
+  <si>
+    <t>Sample Value 33</t>
+  </si>
+  <si>
+    <t>Sample Value 34</t>
+  </si>
+  <si>
+    <t>Sample Value 35</t>
+  </si>
+  <si>
+    <t>Sample Value 39</t>
+  </si>
+  <si>
+    <t>Sample Value 40</t>
+  </si>
+  <si>
+    <t>Sample Value 45</t>
+  </si>
+  <si>
+    <t>Sample Value 46</t>
+  </si>
+  <si>
+    <t>Sample Value 47</t>
+  </si>
+  <si>
+    <t>SuborgCode</t>
+  </si>
+  <si>
+    <t>TransactionNo</t>
+  </si>
+  <si>
+    <t>TransactionDate</t>
+  </si>
+  <si>
+    <t>Suborg</t>
+  </si>
+  <si>
+    <t>SampleEntit</t>
+  </si>
+  <si>
+    <t>SampleEnti</t>
+  </si>
+  <si>
+    <t>SampleEntitt</t>
+  </si>
+  <si>
+    <t>Organization hierarchy</t>
+  </si>
+  <si>
+    <t>CTO</t>
+  </si>
+  <si>
+    <t>CMO</t>
+  </si>
+  <si>
+    <t>STM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub </t>
+  </si>
+  <si>
+    <t>TO</t>
+  </si>
+  <si>
+    <t>DIR</t>
+  </si>
+  <si>
+    <t>CE</t>
   </si>
 </sst>
 </file>
@@ -554,7 +687,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -577,6 +710,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -899,25 +1033,25 @@
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>132</v>
       </c>
       <c r="H1" s="4"/>
     </row>
@@ -926,22 +1060,22 @@
         <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="F2" t="s">
         <v>134</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" t="s">
         <v>135</v>
-      </c>
-      <c r="F2" t="s">
-        <v>136</v>
-      </c>
-      <c r="G2" t="s">
-        <v>137</v>
       </c>
       <c r="H2" s="3"/>
     </row>
@@ -950,22 +1084,22 @@
         <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="F3" t="s">
         <v>139</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" t="s">
         <v>140</v>
-      </c>
-      <c r="F3" t="s">
-        <v>141</v>
-      </c>
-      <c r="G3" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1164,16 +1298,16 @@
         <v>17</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F1" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="12" t="s">
-        <v>40</v>
-      </c>
       <c r="H1" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1190,10 +1324,10 @@
         <v>30</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>22</v>
@@ -1214,10 +1348,10 @@
         <v>30</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>24</v>
@@ -1238,10 +1372,10 @@
         <v>30</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>24</v>
@@ -1270,16 +1404,16 @@
         <v>26</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E6" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>37</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>39</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>24</v>
@@ -1300,10 +1434,10 @@
         <v>30</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>24</v>
@@ -1324,10 +1458,10 @@
         <v>30</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>22</v>
@@ -1356,16 +1490,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.140625" customWidth="1"/>
@@ -1377,7 +1511,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>15</v>
@@ -1389,19 +1523,19 @@
         <v>17</v>
       </c>
       <c r="E1" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="H1" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>46</v>
-      </c>
       <c r="I1" s="15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1409,19 +1543,19 @@
         <v>22</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>76</v>
+        <v>142</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>24</v>
@@ -1439,16 +1573,16 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>77</v>
+        <v>143</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>22</v>
@@ -1466,16 +1600,16 @@
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>78</v>
+        <v>144</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>24</v>
@@ -1493,16 +1627,16 @@
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>79</v>
+        <v>145</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>24</v>
@@ -1520,16 +1654,16 @@
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>80</v>
+        <v>146</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>24</v>
@@ -1547,16 +1681,16 @@
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>81</v>
+        <v>147</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>24</v>
@@ -1586,19 +1720,19 @@
         <v>22</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>82</v>
+        <v>148</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>24</v>
@@ -1616,16 +1750,16 @@
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>83</v>
+        <v>149</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>22</v>
@@ -1643,16 +1777,16 @@
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>84</v>
+        <v>150</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G11" s="10" t="s">
         <v>24</v>
@@ -1670,16 +1804,16 @@
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>85</v>
+        <v>151</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>24</v>
@@ -1693,47 +1827,35 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B13" s="10"/>
-      <c r="C13" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>24</v>
-      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="10"/>
+        <v>22</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>64</v>
+      </c>
       <c r="C14" s="10" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>87</v>
+        <v>152</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>24</v>
@@ -1751,25 +1873,25 @@
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="10" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>88</v>
+        <v>153</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1778,16 +1900,16 @@
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>89</v>
+        <v>154</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>24</v>
@@ -1805,16 +1927,16 @@
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="10" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>90</v>
+        <v>155</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G17" s="10" t="s">
         <v>24</v>
@@ -1832,16 +1954,16 @@
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="10" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>24</v>
@@ -1855,35 +1977,47 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
+      <c r="C19" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>66</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B20" s="10"/>
       <c r="C20" s="10" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>92</v>
+        <v>158</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G20" s="10" t="s">
         <v>24</v>
@@ -1901,70 +2035,58 @@
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="14" t="s">
         <v>30</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>93</v>
+        <v>159</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B22" s="10"/>
-      <c r="C22" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H22" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>24</v>
-      </c>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="10"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>70</v>
+      </c>
       <c r="C23" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D23" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>95</v>
+        <v>160</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G23" s="10" t="s">
         <v>24</v>
@@ -1982,16 +2104,16 @@
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="10" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>96</v>
+        <v>161</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>24</v>
@@ -2009,16 +2131,16 @@
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="14" t="s">
         <v>30</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>97</v>
+        <v>162</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G25" s="10" t="s">
         <v>24</v>
@@ -2036,25 +2158,25 @@
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="10" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D26" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>98</v>
+        <v>163</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -2063,16 +2185,16 @@
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="D27" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>99</v>
+        <v>164</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G27" s="10" t="s">
         <v>24</v>
@@ -2090,16 +2212,16 @@
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="10" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D28" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>100</v>
+        <v>165</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G28" s="10" t="s">
         <v>24</v>
@@ -2117,16 +2239,16 @@
       </c>
       <c r="B29" s="10"/>
       <c r="C29" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D29" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="14" t="s">
         <v>30</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>101</v>
+        <v>166</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G29" s="10" t="s">
         <v>24</v>
@@ -2140,47 +2262,35 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B30" s="10"/>
-      <c r="C30" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H30" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I30" s="10" t="s">
-        <v>24</v>
-      </c>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="10"/>
+        <v>22</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>72</v>
+      </c>
       <c r="C31" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D31" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>103</v>
+        <v>167</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G31" s="10" t="s">
         <v>24</v>
@@ -2194,35 +2304,47 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
+      <c r="C32" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>72</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B33" s="10"/>
       <c r="C33" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D33" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D33" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>104</v>
+        <v>169</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G33" s="10" t="s">
         <v>24</v>
@@ -2240,16 +2362,16 @@
       </c>
       <c r="B34" s="10"/>
       <c r="C34" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D34" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>105</v>
+        <v>170</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G34" s="10" t="s">
         <v>24</v>
@@ -2267,16 +2389,16 @@
       </c>
       <c r="B35" s="10"/>
       <c r="C35" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D35" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>106</v>
+        <v>171</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G35" s="10" t="s">
         <v>24</v>
@@ -2290,463 +2412,16 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B36" s="10"/>
-      <c r="C36" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="F36" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I36" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="F37" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G37" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H37" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I37" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="F38" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I38" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="D39" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E39" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="F39" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G39" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H39" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I39" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="F40" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G40" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I40" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E41" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="F41" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G41" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H41" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I41" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="F42" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G42" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H42" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I42" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="10"/>
-      <c r="I43" s="10"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="F44" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G44" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H44" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I44" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B45" s="10"/>
-      <c r="C45" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D45" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="F45" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G45" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H45" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I45" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B46" s="10"/>
-      <c r="C46" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D46" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="F46" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G46" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H46" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I46" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B47" s="10"/>
-      <c r="C47" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D47" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="F47" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G47" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H47" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I47" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="F48" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G48" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H48" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I48" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B49" s="10"/>
-      <c r="C49" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D49" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E49" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="F49" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G49" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H49" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I49" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D50" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="F50" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G50" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H50" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I50" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D51" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E51" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="F51" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G51" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H51" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I51" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B52" s="10"/>
-      <c r="C52" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E52" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="F52" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G52" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H52" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I52" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B53" s="10"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10"/>
-      <c r="G53" s="10"/>
-      <c r="H53" s="10"/>
-      <c r="I53" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2755,26 +2430,341 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="75.140625" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
+    <row r="1" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2786,7 +2776,7 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2804,7 +2794,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>15</v>
@@ -2816,19 +2806,19 @@
         <v>17</v>
       </c>
       <c r="E1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>46</v>
-      </c>
       <c r="I1" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2836,19 +2826,19 @@
         <v>22</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>24</v>
@@ -2866,16 +2856,16 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>22</v>
@@ -2893,16 +2883,16 @@
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>24</v>
@@ -2920,16 +2910,16 @@
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>24</v>
@@ -2947,16 +2937,16 @@
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>24</v>
@@ -2974,16 +2964,16 @@
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>24</v>
@@ -3013,19 +3003,19 @@
         <v>22</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>24</v>
@@ -3043,16 +3033,16 @@
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>22</v>
@@ -3070,16 +3060,16 @@
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G11" s="10" t="s">
         <v>24</v>
@@ -3097,16 +3087,16 @@
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>24</v>
@@ -3124,16 +3114,16 @@
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>24</v>
@@ -3151,16 +3141,16 @@
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>24</v>
@@ -3178,16 +3168,16 @@
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>24</v>
@@ -3205,16 +3195,16 @@
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>24</v>
@@ -3232,16 +3222,16 @@
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G17" s="10" t="s">
         <v>24</v>
@@ -3259,16 +3249,16 @@
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>24</v>
@@ -3298,19 +3288,19 @@
         <v>22</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G20" s="10" t="s">
         <v>24</v>
@@ -3328,16 +3318,16 @@
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G21" s="10" t="s">
         <v>22</v>
@@ -3355,16 +3345,16 @@
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G22" s="10" t="s">
         <v>24</v>
@@ -3382,16 +3372,16 @@
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G23" s="10" t="s">
         <v>24</v>
@@ -3409,16 +3399,16 @@
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>24</v>
@@ -3436,16 +3426,16 @@
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D25" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G25" s="10" t="s">
         <v>24</v>
@@ -3463,16 +3453,16 @@
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D26" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>24</v>
@@ -3490,16 +3480,16 @@
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D27" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G27" s="10" t="s">
         <v>24</v>
@@ -3517,16 +3507,16 @@
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D28" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G28" s="10" t="s">
         <v>24</v>
@@ -3544,16 +3534,16 @@
       </c>
       <c r="B29" s="10"/>
       <c r="C29" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D29" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G29" s="10" t="s">
         <v>24</v>
@@ -3571,16 +3561,16 @@
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G30" s="10" t="s">
         <v>24</v>
@@ -3598,16 +3588,16 @@
       </c>
       <c r="B31" s="10"/>
       <c r="C31" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G31" s="10" t="s">
         <v>24</v>
@@ -3637,19 +3627,19 @@
         <v>22</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G33" s="10" t="s">
         <v>24</v>
@@ -3667,16 +3657,16 @@
       </c>
       <c r="B34" s="10"/>
       <c r="C34" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G34" s="10" t="s">
         <v>24</v>
@@ -3694,16 +3684,16 @@
       </c>
       <c r="B35" s="10"/>
       <c r="C35" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G35" s="10" t="s">
         <v>24</v>
@@ -3719,16 +3709,16 @@
       </c>
       <c r="B36" s="10"/>
       <c r="C36" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D36" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G36" s="10" t="s">
         <v>22</v>
@@ -3744,13 +3734,13 @@
       </c>
       <c r="B37" s="10"/>
       <c r="C37" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
@@ -3763,13 +3753,13 @@
       </c>
       <c r="B38" s="10"/>
       <c r="C38" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D38" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
@@ -3782,13 +3772,13 @@
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
@@ -3801,13 +3791,13 @@
       </c>
       <c r="B40" s="10"/>
       <c r="C40" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D40" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F40" s="10"/>
       <c r="G40" s="10"/>
@@ -3820,13 +3810,13 @@
       </c>
       <c r="B41" s="10"/>
       <c r="C41" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D41" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
@@ -3839,13 +3829,13 @@
       </c>
       <c r="B42" s="10"/>
       <c r="C42" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
@@ -3870,19 +3860,19 @@
         <v>22</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D44" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G44" s="10"/>
       <c r="H44" s="10"/>
@@ -3894,16 +3884,16 @@
       </c>
       <c r="B45" s="10"/>
       <c r="C45" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D45" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G45" s="10"/>
       <c r="H45" s="10"/>
@@ -3915,16 +3905,16 @@
       </c>
       <c r="B46" s="10"/>
       <c r="C46" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G46" s="10"/>
       <c r="H46" s="10"/>
@@ -3936,16 +3926,16 @@
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D47" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G47" s="10"/>
       <c r="H47" s="10"/>
@@ -3957,13 +3947,13 @@
       </c>
       <c r="B48" s="10"/>
       <c r="C48" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D48" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F48" s="10"/>
       <c r="G48" s="10"/>
@@ -3976,16 +3966,16 @@
       </c>
       <c r="B49" s="10"/>
       <c r="C49" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D49" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G49" s="10"/>
       <c r="H49" s="10"/>
@@ -3997,13 +3987,13 @@
       </c>
       <c r="B50" s="10"/>
       <c r="C50" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D50" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F50" s="10"/>
       <c r="G50" s="10"/>
@@ -4016,13 +4006,13 @@
       </c>
       <c r="B51" s="10"/>
       <c r="C51" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D51" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F51" s="10"/>
       <c r="G51" s="10"/>
@@ -4035,13 +4025,13 @@
       </c>
       <c r="B52" s="10"/>
       <c r="C52" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D52" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F52" s="10"/>
       <c r="G52" s="10"/>
@@ -4064,4 +4054,56 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>186</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated stable code for smoke testing
</commit_message>
<xml_diff>
--- a/TestingFramework/TestData/testInput.xlsx
+++ b/TestingFramework/TestData/testInput.xlsx
@@ -4,20 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="345" windowWidth="14805" windowHeight="7770" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Organisation" sheetId="12" r:id="rId1"/>
     <sheet name="Process" sheetId="11" r:id="rId2"/>
     <sheet name="Entity" sheetId="13" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="14" r:id="rId4"/>
+    <sheet name="BulkProject" sheetId="15" r:id="rId5"/>
+    <sheet name="RandomDelete" sheetId="16" r:id="rId6"/>
+    <sheet name="bulkpro" sheetId="17" r:id="rId7"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3252" uniqueCount="833">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3492" uniqueCount="1042">
   <si>
     <t>Hyderabad</t>
   </si>
@@ -2516,13 +2519,1025 @@
   </si>
   <si>
     <t>subMod1,subMod2,submod3,submod4,submod5,submod6,submod7,submod8,submod9</t>
+  </si>
+  <si>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>Module Name</t>
+  </si>
+  <si>
+    <t>Sub-Module Name</t>
+  </si>
+  <si>
+    <t>Kagami-Project-Name_1</t>
+  </si>
+  <si>
+    <t>Project-Module_1, Project-Module_2, Project-Module_3</t>
+  </si>
+  <si>
+    <t>SubModule1, SubModule2, SubModule3</t>
+  </si>
+  <si>
+    <t>Kagami-Project-Name_2</t>
+  </si>
+  <si>
+    <t>Project-Module_1, Project-Module_2, Project-Module_4</t>
+  </si>
+  <si>
+    <t>SubModule1, SubModule2, SubModule4</t>
+  </si>
+  <si>
+    <t>Process1, Process2, Process3, Process5</t>
+  </si>
+  <si>
+    <t>Kagami-Project-Name_3</t>
+  </si>
+  <si>
+    <t>SubModule1, SubModule2, SubModule5</t>
+  </si>
+  <si>
+    <t>Process1, Process2, Process3, Process6</t>
+  </si>
+  <si>
+    <t>Kagami-Project-Name_4</t>
+  </si>
+  <si>
+    <t>Project-Module_1, Project-Module_2, Project-Module_6</t>
+  </si>
+  <si>
+    <t>Process1, Process2, Process3, Process7</t>
+  </si>
+  <si>
+    <t>Kagami-Project-Name_5</t>
+  </si>
+  <si>
+    <t>Project-Module_1, Project-Module_2, Project-Module_7</t>
+  </si>
+  <si>
+    <t>SubModule1, SubModule2, SubModule7</t>
+  </si>
+  <si>
+    <t>Kagami-Project-Name_6</t>
+  </si>
+  <si>
+    <t>SubModule1, SubModule2, SubModule8</t>
+  </si>
+  <si>
+    <t>Process1, Process2, Process3, Process9</t>
+  </si>
+  <si>
+    <t>Kagami-Project-Name_7</t>
+  </si>
+  <si>
+    <t>Project-Module_1, Project-Module_2, Project-Module_9</t>
+  </si>
+  <si>
+    <t>Process1, Process2, Process3, Process10</t>
+  </si>
+  <si>
+    <t>Kagami-Project-Name_8</t>
+  </si>
+  <si>
+    <t>Project-Module_1, Project-Module_2, Project-Module_10</t>
+  </si>
+  <si>
+    <t>Process1, Process2, Process3, Process11</t>
+  </si>
+  <si>
+    <t>Kagami-Project-Name_9</t>
+  </si>
+  <si>
+    <t>Project-Module_1, Project-Module_2, Project-Module_11</t>
+  </si>
+  <si>
+    <t>SubModule1, SubModule2, SubModule11</t>
+  </si>
+  <si>
+    <t>Kagami-Project-Name_10</t>
+  </si>
+  <si>
+    <t>Project-Module_1, Project-Module_2, Project-Module_12</t>
+  </si>
+  <si>
+    <t>SubModule1, SubModule2, SubModule12</t>
+  </si>
+  <si>
+    <t>Kagami-Project-Name_11</t>
+  </si>
+  <si>
+    <t>Project-Module_1, Project-Module_2, Project-Module_13</t>
+  </si>
+  <si>
+    <t>SubModule1, SubModule2, SubModule13</t>
+  </si>
+  <si>
+    <t>Process1, Process2, Process3, Process14</t>
+  </si>
+  <si>
+    <t>Kagami-Project-Name_12</t>
+  </si>
+  <si>
+    <t>Project-Module_1, Project-Module_2, Project-Module_14</t>
+  </si>
+  <si>
+    <t>SubModule1, SubModule2, SubModule14</t>
+  </si>
+  <si>
+    <t>Process1, Process2, Process3, Process15</t>
+  </si>
+  <si>
+    <t>Kagami-Project-Name_13</t>
+  </si>
+  <si>
+    <t>Project-Module_1, Project-Module_2, Project-Module_15</t>
+  </si>
+  <si>
+    <t>Process1, Process2, Process3, Process16</t>
+  </si>
+  <si>
+    <t>Kagami-Project-Name_14</t>
+  </si>
+  <si>
+    <t>Project-Module_1, Project-Module_2, Project-Module_16</t>
+  </si>
+  <si>
+    <t>Process1, Process2, Process3, Process17</t>
+  </si>
+  <si>
+    <t>Kagami-Project-Name_15</t>
+  </si>
+  <si>
+    <t>Project-Module_1, Project-Module_2, Project-Module_17</t>
+  </si>
+  <si>
+    <t>SubModule1, SubModule2, SubModule17</t>
+  </si>
+  <si>
+    <t>Process1, Process2, Process3, Process18</t>
+  </si>
+  <si>
+    <t>Kagami-Project-Name_16</t>
+  </si>
+  <si>
+    <t>Project-Module_1, Project-Module_2, Project-Module_18</t>
+  </si>
+  <si>
+    <t>SubModule1, SubModule2, SubModule18</t>
+  </si>
+  <si>
+    <t>Kagami-Project-Name_17</t>
+  </si>
+  <si>
+    <t>Project-Module_1, Project-Module_2, Project-Module_19</t>
+  </si>
+  <si>
+    <t>SubModule1, SubModule2, SubModule19</t>
+  </si>
+  <si>
+    <t>Kagami-Project-Name_18</t>
+  </si>
+  <si>
+    <t>Project-Module_1, Project-Module_2, Project-Module_20</t>
+  </si>
+  <si>
+    <t>SubModule1, SubModule2, SubModule20</t>
+  </si>
+  <si>
+    <t>Kagami-Project-Name_19</t>
+  </si>
+  <si>
+    <t>Project-Module_1, Project-Module_2, Project-Module_21</t>
+  </si>
+  <si>
+    <t>SubModule1, SubModule2, SubModule21</t>
+  </si>
+  <si>
+    <t>Kagami-Project-Name_20</t>
+  </si>
+  <si>
+    <t>SubModule1, SubModule2, SubModule22</t>
+  </si>
+  <si>
+    <t>Process1, Process2, Process3, Process23</t>
+  </si>
+  <si>
+    <t>Kagami-Project-Name_21</t>
+  </si>
+  <si>
+    <t>SubModule1, SubModule2, SubModule23</t>
+  </si>
+  <si>
+    <t>Process1, Process2, Process3, Process24</t>
+  </si>
+  <si>
+    <t>Kagami-Project-Name_22</t>
+  </si>
+  <si>
+    <t>SubModule1, SubModule2, SubModule24</t>
+  </si>
+  <si>
+    <t>Process1, Process2, Process3, Process25</t>
+  </si>
+  <si>
+    <t>Kagami-Project-Name_23</t>
+  </si>
+  <si>
+    <t>SubModule1, SubModule2, SubModule25</t>
+  </si>
+  <si>
+    <t>Process1, Process2, Process3, Process26</t>
+  </si>
+  <si>
+    <t>Kagami-Project-Name_24</t>
+  </si>
+  <si>
+    <t>Project-Module_1, Project-Module_2, Project-Module_26</t>
+  </si>
+  <si>
+    <t>SubModule1, SubModule2, SubModule26</t>
+  </si>
+  <si>
+    <t>Process1, Process2, Process3, Process27</t>
+  </si>
+  <si>
+    <t>Kagami-Project-Name_25</t>
+  </si>
+  <si>
+    <t>Project-Module_1, Project-Module_2, Project-Module_27</t>
+  </si>
+  <si>
+    <t>SubModule1, SubModule2, SubModule27</t>
+  </si>
+  <si>
+    <t>Process1, Process2, Process3, Process28</t>
+  </si>
+  <si>
+    <t>Kagami-Project-Name_26</t>
+  </si>
+  <si>
+    <t>Project-Module_1, Project-Module_2, Project-Module_28</t>
+  </si>
+  <si>
+    <t>SubModule1, SubModule2, SubModule28</t>
+  </si>
+  <si>
+    <t>Process1, Process2, Process3, Process29</t>
+  </si>
+  <si>
+    <t>Kagami-Project-Name_27</t>
+  </si>
+  <si>
+    <t>Project-Module_1, Project-Module_2, Project-Module_29</t>
+  </si>
+  <si>
+    <t>SubModule1, SubModule2, SubModule29</t>
+  </si>
+  <si>
+    <t>Process1, Process2, Process3, Process30</t>
+  </si>
+  <si>
+    <t>Kagami-Project-Name_28</t>
+  </si>
+  <si>
+    <t>Project-Module_1, Project-Module_2, Project-Module_30</t>
+  </si>
+  <si>
+    <t>Process1, Process2, Process3, Process31</t>
+  </si>
+  <si>
+    <t>Kagami-Project-Name_29</t>
+  </si>
+  <si>
+    <t>Project-Module_1, Project-Module_2, Project-Module_31</t>
+  </si>
+  <si>
+    <t>Process1, Process2, Process3, Process32</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Process1, Process2, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Process3, Process4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SubModule1,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> SubModule2, SubModule4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Project-Module_1, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Project-Module_2,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Project-Module_5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">SubModule1, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SubModule2, SubModule6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Process1,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Process2, Process3, Process8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Project-Module_1, Project-Module_2,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Project-Module_8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SubModule1, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SubModule2,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> SubModule9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SubModule1, SubModule2, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SubModule10</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Process1, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Process2,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Process3, Process12</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Process1, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Process2, Process3, Process13</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SubModule1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, SubModule2, SubModule15</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SubModule1,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> SubModule2, SubModule16</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Process1, Process2, Process3,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Process19</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Process1,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Process2, Process3, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Process20</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Process1, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Process2, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Process3, Process21</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Process1, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Process2,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Process3, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Process22</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Project-Module_1,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Project-Module_2, Project-Module_22</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Project-Module_1, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Project-Module_2, Project-Module_23</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Project-Module_1,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Project-Module_2,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Project-Module_24</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Project-Module_1, Project-Module_2,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Project-Module_25</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SubModule1, SubModule2,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> SubModule30</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SubModule1,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> SubModule2, SubModule31</t>
+    </r>
+  </si>
+  <si>
+    <t>Save drivingLicenseDetails</t>
+  </si>
+  <si>
+    <t>Process1, Process2, Process3</t>
+  </si>
+  <si>
+    <t>Process1, Process2, Process4</t>
+  </si>
+  <si>
+    <t>Select Module</t>
+  </si>
+  <si>
+    <t>Module_1</t>
+  </si>
+  <si>
+    <t>Module_2</t>
+  </si>
+  <si>
+    <t>Select Sub-Module</t>
+  </si>
+  <si>
+    <t>Module_1, Module_2,Module_3</t>
+  </si>
+  <si>
+    <t>SubModule1</t>
+  </si>
+  <si>
+    <t>Module_1, Module_2,Module_4</t>
+  </si>
+  <si>
+    <t>Module_1, Module_2,Module_5</t>
+  </si>
+  <si>
+    <t>Module_4</t>
+  </si>
+  <si>
+    <t>Module_13</t>
+  </si>
+  <si>
+    <t>Module_22</t>
+  </si>
+  <si>
+    <t>SubModule2</t>
+  </si>
+  <si>
+    <t>SubModule5</t>
+  </si>
+  <si>
+    <t>SubModule11</t>
+  </si>
+  <si>
+    <t>SubModule22</t>
+  </si>
+  <si>
+    <t>Module_21, Module_22,Module_23</t>
+  </si>
+  <si>
+    <t>SubModule21, SubModule22, SubModule23</t>
+  </si>
+  <si>
+    <t>SubModule31, SubModule32, SubModule33</t>
+  </si>
+  <si>
+    <t>SubModule33</t>
+  </si>
+  <si>
+    <t>Module_31, Module_32,Module_33</t>
+  </si>
+  <si>
+    <t>Module_11, Module_12,Module_13</t>
+  </si>
+  <si>
+    <t>SubModule11, SubModule12, SubModule13</t>
+  </si>
+  <si>
+    <t>Process11, Process12, Process13</t>
+  </si>
+  <si>
+    <t>Process21, Process22, Process23</t>
+  </si>
+  <si>
+    <t>Module_41, Module_42,Module_43</t>
+  </si>
+  <si>
+    <t>Module_51, Module_52,Module_53</t>
+  </si>
+  <si>
+    <t>Module_61, Module_62,Module_63</t>
+  </si>
+  <si>
+    <t>Module_71, Module_72,Module_73</t>
+  </si>
+  <si>
+    <t>Module_81, Module_82,Module_83</t>
+  </si>
+  <si>
+    <t>Module_91, Module_92,Module_93</t>
+  </si>
+  <si>
+    <t>Module_101, Module_102,Module_103</t>
+  </si>
+  <si>
+    <t>Module_111, Module_112,Module_113</t>
+  </si>
+  <si>
+    <t>Module_121, Module_122,Module_123</t>
+  </si>
+  <si>
+    <t>Module_131, Module_132,Module_133</t>
+  </si>
+  <si>
+    <t>Module_141, Module_142,Module_143</t>
+  </si>
+  <si>
+    <t>Module_151, Module_152,Module_153</t>
+  </si>
+  <si>
+    <t>Module_33</t>
+  </si>
+  <si>
+    <t>Module_42</t>
+  </si>
+  <si>
+    <t>Module_52</t>
+  </si>
+  <si>
+    <t>Module_63</t>
+  </si>
+  <si>
+    <t>Module_71</t>
+  </si>
+  <si>
+    <t>Module_83</t>
+  </si>
+  <si>
+    <t>Module_91</t>
+  </si>
+  <si>
+    <t>Module_101</t>
+  </si>
+  <si>
+    <t>Module_111</t>
+  </si>
+  <si>
+    <t>Module_121</t>
+  </si>
+  <si>
+    <t>Module_132</t>
+  </si>
+  <si>
+    <t>Module_141</t>
+  </si>
+  <si>
+    <t>Module_151</t>
+  </si>
+  <si>
+    <t>SubModule41, SubModule42, SubModule43</t>
+  </si>
+  <si>
+    <t>SubModule51, SubModule52, SubModule53</t>
+  </si>
+  <si>
+    <t>SubModule61, SubModule62, SubModule63</t>
+  </si>
+  <si>
+    <t>SubModule71, SubModule72, SubModule73</t>
+  </si>
+  <si>
+    <t>SubModule81, SubModule82, SubModule83</t>
+  </si>
+  <si>
+    <t>SubModule91, SubModule92, SubModule93</t>
+  </si>
+  <si>
+    <t>SubModule101, SubModule102, SubModule103</t>
+  </si>
+  <si>
+    <t>SubModule121, SubModule122, SubModule123</t>
+  </si>
+  <si>
+    <t>SubModule111, SubModule112, SubModule113</t>
+  </si>
+  <si>
+    <t>SubModule131, SubModule132, SubModule133</t>
+  </si>
+  <si>
+    <t>SubModule141, SubModule142, SubModule143</t>
+  </si>
+  <si>
+    <t>SubModule151, SubModule152, SubModule153</t>
+  </si>
+  <si>
+    <t>SubModule42</t>
+  </si>
+  <si>
+    <t>SubModule51</t>
+  </si>
+  <si>
+    <t>SubModule61</t>
+  </si>
+  <si>
+    <t>SubModule72</t>
+  </si>
+  <si>
+    <t>SubModule83</t>
+  </si>
+  <si>
+    <t>SubModule93</t>
+  </si>
+  <si>
+    <t>SubModule101</t>
+  </si>
+  <si>
+    <t>SubModule112</t>
+  </si>
+  <si>
+    <t>SubModule123</t>
+  </si>
+  <si>
+    <t>SubModule131</t>
+  </si>
+  <si>
+    <t>SubModule142</t>
+  </si>
+  <si>
+    <t>SubModule153</t>
+  </si>
+  <si>
+    <t>Process31, Process32, Process34</t>
+  </si>
+  <si>
+    <t>Process41, Process42, Process43</t>
+  </si>
+  <si>
+    <t>Process51, Process52, Process53</t>
+  </si>
+  <si>
+    <t>Process61, Process62, Process63</t>
+  </si>
+  <si>
+    <t>Process71, Process72, Process73</t>
+  </si>
+  <si>
+    <t>Process81, Process82, Process83</t>
+  </si>
+  <si>
+    <t>Process91, Process92, Process93</t>
+  </si>
+  <si>
+    <t>Process101, Process102, Process103</t>
+  </si>
+  <si>
+    <t>Process111, Process112, Process113</t>
+  </si>
+  <si>
+    <t>Process121, Process122, Process133</t>
+  </si>
+  <si>
+    <t>Process131, Process132, Process133</t>
+  </si>
+  <si>
+    <t>Process141, Process142, Process143</t>
+  </si>
+  <si>
+    <t>Process151, Process152, Process153</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2577,8 +3592,22 @@
       <name val="Trebuchet MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2600,6 +3629,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2656,7 +3691,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2717,6 +3752,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3348,7 +4388,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -4117,13 +5157,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K575"/>
   <sheetViews>
-    <sheetView topLeftCell="A186" workbookViewId="0">
-      <selection activeCell="C198" sqref="C198"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.140625" style="11" customWidth="1"/>
     <col min="3" max="3" width="31.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" style="11" customWidth="1"/>
@@ -4263,7 +5303,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>953</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -18545,4 +19585,896 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="28"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>833</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>834</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>956</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>835</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>959</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>836</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>960</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>957</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>838</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>961</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>839</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>962</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>964</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>841</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>967</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>843</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>963</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>958</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>844</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>968</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>955</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="31"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>833</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>834</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>835</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>836</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>837</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>838</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>839</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>840</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>932</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>843</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>933</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>844</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>846</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>847</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>934</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>849</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>850</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>851</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
+        <v>852</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>936</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>853</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
+        <v>855</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>856</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>937</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="30" t="s">
+        <v>858</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>859</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>938</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
+        <v>861</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>862</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>863</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="30" t="s">
+        <v>864</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>865</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>866</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="30" t="s">
+        <v>867</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>868</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>869</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="30" t="s">
+        <v>871</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>872</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>873</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="30" t="s">
+        <v>875</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>876</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>941</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
+        <v>878</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>879</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>942</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="30" t="s">
+        <v>881</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>882</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>883</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
+        <v>885</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>886</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>887</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="30" t="s">
+        <v>888</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>889</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>890</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="30" t="s">
+        <v>891</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>892</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>893</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="30" t="s">
+        <v>894</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>895</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>896</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="30" t="s">
+        <v>897</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>947</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>898</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="30" t="s">
+        <v>900</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>948</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>901</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="30" t="s">
+        <v>903</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>949</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>904</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="30" t="s">
+        <v>906</v>
+      </c>
+      <c r="B24" s="32" t="s">
+        <v>950</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>907</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
+        <v>909</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>910</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>911</v>
+      </c>
+      <c r="D25" s="30" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="32" t="s">
+        <v>913</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>914</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>915</v>
+      </c>
+      <c r="D26" s="30" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="32" t="s">
+        <v>917</v>
+      </c>
+      <c r="B27" s="30" t="s">
+        <v>918</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>919</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="32" t="s">
+        <v>921</v>
+      </c>
+      <c r="B28" s="30" t="s">
+        <v>922</v>
+      </c>
+      <c r="C28" s="30" t="s">
+        <v>923</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="30" t="s">
+        <v>925</v>
+      </c>
+      <c r="B29" s="30" t="s">
+        <v>926</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>951</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="30" t="s">
+        <v>928</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>929</v>
+      </c>
+      <c r="C30" s="32" t="s">
+        <v>952</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>930</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="28"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>833</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>834</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>956</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>835</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>959</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>836</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>976</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>965</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>977</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>969</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>839</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>971</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>966</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>972</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>970</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>843</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>975</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>992</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>973</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>974</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>846</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>980</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>993</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>1017</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>849</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>981</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>994</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>1006</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>1018</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
+        <v>852</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>982</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>995</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>1019</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
+        <v>855</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>983</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>996</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>1008</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>1020</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="30" t="s">
+        <v>858</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>984</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>997</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>1009</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>1021</v>
+      </c>
+      <c r="F9" s="30" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
+        <v>861</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>985</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>998</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>1010</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>1022</v>
+      </c>
+      <c r="F10" s="30" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="30" t="s">
+        <v>864</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>986</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>999</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>1011</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>1023</v>
+      </c>
+      <c r="F11" s="30" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="30" t="s">
+        <v>867</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>987</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>1024</v>
+      </c>
+      <c r="F12" s="30" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="30" t="s">
+        <v>871</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>988</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>1001</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>1012</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>1025</v>
+      </c>
+      <c r="F13" s="30" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="30" t="s">
+        <v>875</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>989</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>1002</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>1014</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>1026</v>
+      </c>
+      <c r="F14" s="30" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
+        <v>878</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>990</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>1003</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>1027</v>
+      </c>
+      <c r="F15" s="30" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="30" t="s">
+        <v>881</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>991</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>1016</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>1028</v>
+      </c>
+      <c r="F16" s="30" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added All the smoke test code till deployment
</commit_message>
<xml_diff>
--- a/TestingFramework/TestData/testInput.xlsx
+++ b/TestingFramework/TestData/testInput.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650"/>
+    <workbookView xWindow="240" yWindow="645" windowWidth="14805" windowHeight="7470" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="studiologin" sheetId="18" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
   <si>
     <t>Yes</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Create</t>
   </si>
   <si>
-    <t>formTemplate</t>
-  </si>
-  <si>
     <t>UI Template</t>
   </si>
   <si>
@@ -110,21 +107,12 @@
     <t>subMod1</t>
   </si>
   <si>
-    <t>subMod2</t>
-  </si>
-  <si>
     <t>Org</t>
   </si>
   <si>
     <t>Head</t>
   </si>
   <si>
-    <t>Reporties</t>
-  </si>
-  <si>
-    <t>Kagami</t>
-  </si>
-  <si>
     <t>CEO</t>
   </si>
   <si>
@@ -161,15 +149,9 @@
     <t>Process100</t>
   </si>
   <si>
-    <t>Process101</t>
-  </si>
-  <si>
     <t>Save Process100</t>
   </si>
   <si>
-    <t>Save Process101</t>
-  </si>
-  <si>
     <t>Save drivingLicenseDetails</t>
   </si>
   <si>
@@ -209,9 +191,6 @@
     <t>past</t>
   </si>
   <si>
-    <t>subMod1,subMod2</t>
-  </si>
-  <si>
     <t>DemoProject</t>
   </si>
   <si>
@@ -239,7 +218,7 @@
     <t>Child1,Child2</t>
   </si>
   <si>
-    <t>DrivingLeccDetail</t>
+    <t>riskk</t>
   </si>
 </sst>
 </file>
@@ -682,7 +661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -690,18 +669,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -711,72 +690,64 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="2"/>
+    <col min="2" max="2" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="11" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -787,10 +758,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,33 +775,33 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>13</v>
@@ -839,7 +810,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>14</v>
@@ -847,157 +818,80 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="7" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="7" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1026,7 +920,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1039,7 +933,7 @@
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1055,19 +949,19 @@
         <v>4</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>6</v>
@@ -1084,22 +978,22 @@
         <v>0</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>1</v>
@@ -1123,7 +1017,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G5" s="7">
         <v>899</v>
@@ -1146,7 +1040,7 @@
         <v>11</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
@@ -1154,7 +1048,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1176,7 +1070,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1187,33 +1081,33 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Suite for EditComponent
</commit_message>
<xml_diff>
--- a/TestingFramework/TestData/testInput.xlsx
+++ b/TestingFramework/TestData/testInput.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="645" windowWidth="14805" windowHeight="7470" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="705" windowWidth="14805" windowHeight="7410" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="studiologin" sheetId="18" r:id="rId1"/>
     <sheet name="Organisation" sheetId="12" r:id="rId2"/>
-    <sheet name="Process" sheetId="11" r:id="rId3"/>
-    <sheet name="Entity" sheetId="19" r:id="rId4"/>
-    <sheet name="dashboard" sheetId="20" r:id="rId5"/>
+    <sheet name="Entity" sheetId="19" r:id="rId3"/>
+    <sheet name="dashboard" sheetId="20" r:id="rId4"/>
+    <sheet name="ProcessAndPolicies" sheetId="21" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="89">
   <si>
     <t>Yes</t>
   </si>
@@ -56,9 +56,6 @@
     <t>notNull</t>
   </si>
   <si>
-    <t>Number</t>
-  </si>
-  <si>
     <t>Process Name</t>
   </si>
   <si>
@@ -146,12 +143,6 @@
     <t>TestProject</t>
   </si>
   <si>
-    <t>Process100</t>
-  </si>
-  <si>
-    <t>Save Process100</t>
-  </si>
-  <si>
     <t>Save drivingLicenseDetails</t>
   </si>
   <si>
@@ -164,9 +155,6 @@
     <t>admin</t>
   </si>
   <si>
-    <t>pcCreate</t>
-  </si>
-  <si>
     <t>EntityName</t>
   </si>
   <si>
@@ -191,34 +179,115 @@
     <t>past</t>
   </si>
   <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>GroupName</t>
+  </si>
+  <si>
+    <t>ChildName</t>
+  </si>
+  <si>
+    <t>Process</t>
+  </si>
+  <si>
+    <t>Process1</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Group1</t>
+  </si>
+  <si>
+    <t>Child1,Child2</t>
+  </si>
+  <si>
+    <t>Process101</t>
+  </si>
+  <si>
+    <t>Save Process101</t>
+  </si>
+  <si>
+    <t>employeeNo,drivingLicenseNo</t>
+  </si>
+  <si>
+    <t>formTemplate</t>
+  </si>
+  <si>
+    <t>Condition &amp; Restrictions</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Japan.employeeNo,not equals,KGM100 and
+Japan.drivingLicenseNo,not equals,1000 and
+Japan.employeeNo,not equals,KGM120 and
+Japan.employeeNo,equals,KGM190</t>
+  </si>
+  <si>
+    <t>Attributes</t>
+  </si>
+  <si>
     <t>DemoProject</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>GroupName</t>
-  </si>
-  <si>
-    <t>ChildName</t>
-  </si>
-  <si>
-    <t>Process</t>
-  </si>
-  <si>
-    <t>Process1</t>
-  </si>
-  <si>
-    <t>Group</t>
-  </si>
-  <si>
-    <t>Group1</t>
-  </si>
-  <si>
-    <t>Child1,Child2</t>
-  </si>
-  <si>
-    <t>riskk</t>
+    <t>EntityType</t>
+  </si>
+  <si>
+    <t>DrivingLicenseDetailess</t>
+  </si>
+  <si>
+    <t>Transaction</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>StateDetailss</t>
+  </si>
+  <si>
+    <t>Master</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Capital</t>
+  </si>
+  <si>
+    <t>Save StateDetails</t>
+  </si>
+  <si>
+    <t>ImmigrationInfos</t>
+  </si>
+  <si>
+    <t>1, 10000</t>
+  </si>
+  <si>
+    <t>passportNumber</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>LowerCase, 1, 1000, Alphanumeric</t>
+  </si>
+  <si>
+    <t>hyderabad1</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>future</t>
+  </si>
+  <si>
+    <t>Save immigrationInfo</t>
   </si>
 </sst>
 </file>
@@ -330,7 +399,9 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -339,7 +410,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -354,9 +425,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,25 +741,25 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -692,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,48 +785,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>29</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -758,169 +837,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -930,10 +868,11 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -943,112 +882,121 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E3" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>52</v>
-      </c>
       <c r="G3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="I3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="J3" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C4" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>40</v>
-      </c>
       <c r="E4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>53</v>
-      </c>
       <c r="G4" s="7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="7"/>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="7"/>
+      <c r="D5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>12</v>
-      </c>
       <c r="E5" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="G5" s="7">
+      <c r="G5" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="7">
         <v>899</v>
       </c>
-      <c r="H5" s="7"/>
       <c r="I5" s="7"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="7"/>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="7"/>
+      <c r="D6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="F6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6" s="7"/>
+      <c r="G6" s="7" t="s">
+        <v>52</v>
+      </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1058,6 +1006,185 @@
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" s="7">
+        <v>9000</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="H12" s="7">
+        <v>3412</v>
+      </c>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1065,7 +1192,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1080,37 +1207,203 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>60</v>
+      <c r="A1" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.140625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="13"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>